<commit_message>
Updates on morphology of galaxies from the data sample
</commit_message>
<xml_diff>
--- a/results/morphology/visual_classification_all.xlsx
+++ b/results/morphology/visual_classification_all.xlsx
@@ -471,14 +471,14 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="1" t="n">
         <v>192481</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -487,44 +487,44 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="1" t="n">
         <v>161191</v>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="1" t="n">
         <v>53237</v>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
@@ -536,21 +536,21 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="1" t="n">
         <v>210809</v>
       </c>
       <c r="B5" t="n">
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -559,11 +559,11 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="1" t="n">
         <v>190256</v>
       </c>
       <c r="B6" t="n">
@@ -573,7 +573,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -586,7 +586,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" s="1" t="n">
         <v>165390</v>
       </c>
       <c r="B7" t="n">
@@ -596,7 +596,7 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -609,7 +609,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" s="1" t="n">
         <v>182930</v>
       </c>
       <c r="B8" t="n">
@@ -622,7 +622,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -632,7 +632,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" s="1" t="n">
         <v>171848</v>
       </c>
       <c r="B9" t="n">
@@ -642,7 +642,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -655,7 +655,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
+      <c r="A10" s="1" t="n">
         <v>197911</v>
       </c>
       <c r="B10" t="n">
@@ -668,7 +668,7 @@
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -678,14 +678,14 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
+      <c r="A11" s="1" t="n">
         <v>57280</v>
       </c>
       <c r="B11" t="n">
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
@@ -694,37 +694,37 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
+      <c r="A12" s="1" t="n">
         <v>175454</v>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
+      <c r="A13" s="1" t="n">
         <v>195892</v>
       </c>
       <c r="B13" t="n">
@@ -734,7 +734,7 @@
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -747,14 +747,14 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
+      <c r="A14" s="1" t="n">
         <v>203821</v>
       </c>
       <c r="B14" t="n">
         <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
@@ -763,14 +763,14 @@
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
+      <c r="A15" s="1" t="n">
         <v>25037</v>
       </c>
       <c r="B15" t="n">
@@ -780,7 +780,7 @@
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
@@ -793,30 +793,30 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
+      <c r="A16" s="1" t="n">
         <v>197884</v>
       </c>
       <c r="B16" t="n">
         <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" t="n">
         <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
+      <c r="A17" s="1" t="n">
         <v>209182</v>
       </c>
       <c r="B17" t="n">
@@ -826,7 +826,7 @@
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
@@ -839,17 +839,17 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
+      <c r="A18" s="1" t="n">
         <v>187812</v>
       </c>
       <c r="B18" t="n">
         <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
@@ -858,18 +858,18 @@
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
+      <c r="A19" s="1" t="n">
         <v>203899</v>
       </c>
       <c r="B19" t="n">
         <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D19" t="n">
         <v>0</v>
@@ -878,24 +878,24 @@
         <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G19" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="n">
+      <c r="A20" s="1" t="n">
         <v>170446</v>
       </c>
       <c r="B20" t="n">
         <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
@@ -904,41 +904,41 @@
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="n">
+      <c r="A21" s="1" t="n">
         <v>191134</v>
       </c>
       <c r="B21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="n">
+      <c r="A22" s="1" t="n">
         <v>210885</v>
       </c>
       <c r="B22" t="n">
         <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D22" t="n">
         <v>0</v>
@@ -947,14 +947,14 @@
         <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G22" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="n">
+      <c r="A23" s="1" t="n">
         <v>186128</v>
       </c>
       <c r="B23" t="n">
@@ -964,7 +964,7 @@
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E23" t="n">
         <v>0</v>
@@ -977,17 +977,17 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="n">
+      <c r="A24" s="1" t="n">
         <v>171592</v>
       </c>
       <c r="B24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
@@ -996,18 +996,18 @@
         <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="n">
+      <c r="A25" s="1" t="n">
         <v>167181</v>
       </c>
       <c r="B25" t="n">
         <v>0</v>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>
@@ -1016,21 +1016,21 @@
         <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="n">
+      <c r="A26" s="1" t="n">
         <v>183858</v>
       </c>
       <c r="B26" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
@@ -1039,21 +1039,21 @@
         <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="n">
+      <c r="A27" s="1" t="n">
         <v>186780</v>
       </c>
       <c r="B27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D27" t="n">
         <v>0</v>
@@ -1065,18 +1065,18 @@
         <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="n">
+      <c r="A28" s="1" t="n">
         <v>155468</v>
       </c>
       <c r="B28" t="n">
         <v>0</v>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D28" t="n">
         <v>0</v>
@@ -1085,14 +1085,14 @@
         <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G28" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="n">
+      <c r="A29" s="1" t="n">
         <v>176606</v>
       </c>
       <c r="B29" t="n">
@@ -1102,20 +1102,20 @@
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F29" t="n">
         <v>0</v>
       </c>
       <c r="G29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="n">
+      <c r="A30" s="1" t="n">
         <v>206907</v>
       </c>
       <c r="B30" t="n">
@@ -1128,7 +1128,7 @@
         <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F30" t="n">
         <v>0</v>
@@ -1138,7 +1138,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="n">
+      <c r="A31" s="1" t="n">
         <v>171849</v>
       </c>
       <c r="B31" t="n">
@@ -1148,7 +1148,7 @@
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E31" t="n">
         <v>0</v>
@@ -1161,17 +1161,17 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="n">
+      <c r="A32" s="1" t="n">
         <v>210620</v>
       </c>
       <c r="B32" t="n">
         <v>0</v>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32" t="n">
         <v>0</v>
@@ -1180,38 +1180,38 @@
         <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="n">
+      <c r="A33" s="1" t="n">
         <v>182126</v>
       </c>
       <c r="B33" t="n">
         <v>0</v>
       </c>
       <c r="C33" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33" t="n">
         <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="n">
+      <c r="A34" s="1" t="n">
         <v>211355</v>
       </c>
       <c r="B34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
@@ -1220,24 +1220,24 @@
         <v>0</v>
       </c>
       <c r="E34" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F34" t="n">
         <v>0</v>
       </c>
       <c r="G34" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="n">
+      <c r="A35" s="1" t="n">
         <v>171816</v>
       </c>
       <c r="B35" t="n">
         <v>0</v>
       </c>
       <c r="C35" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D35" t="n">
         <v>0</v>
@@ -1246,14 +1246,14 @@
         <v>0</v>
       </c>
       <c r="F35" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G35" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="n">
+      <c r="A36" s="1" t="n">
         <v>212998</v>
       </c>
       <c r="B36" t="n">
@@ -1263,7 +1263,7 @@
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E36" t="n">
         <v>0</v>
@@ -1276,14 +1276,14 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="n">
+      <c r="A37" s="1" t="n">
         <v>77693</v>
       </c>
       <c r="B37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C37" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D37" t="n">
         <v>0</v>
@@ -1292,18 +1292,18 @@
         <v>0</v>
       </c>
       <c r="F37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G37" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="n">
+      <c r="A38" s="1" t="n">
         <v>160773</v>
       </c>
       <c r="B38" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
@@ -1318,11 +1318,11 @@
         <v>0</v>
       </c>
       <c r="G38" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="n">
+      <c r="A39" s="1" t="n">
         <v>190245</v>
       </c>
       <c r="B39" t="n">
@@ -1335,7 +1335,7 @@
         <v>0</v>
       </c>
       <c r="E39" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F39" t="n">
         <v>0</v>
@@ -1345,34 +1345,34 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="n">
+      <c r="A40" s="1" t="n">
         <v>189297</v>
       </c>
       <c r="B40" t="n">
         <v>0</v>
       </c>
       <c r="C40" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40" t="n">
         <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="n">
+      <c r="A41" s="1" t="n">
         <v>208432</v>
       </c>
       <c r="B41" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
@@ -1387,11 +1387,11 @@
         <v>0</v>
       </c>
       <c r="G41" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="n">
+      <c r="A42" s="1" t="n">
         <v>214953</v>
       </c>
       <c r="B42" t="n">
@@ -1404,7 +1404,7 @@
         <v>0</v>
       </c>
       <c r="E42" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F42" t="n">
         <v>0</v>
@@ -1414,7 +1414,7 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="n">
+      <c r="A43" s="1" t="n">
         <v>187727</v>
       </c>
       <c r="B43" t="n">
@@ -1424,7 +1424,7 @@
         <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E43" t="n">
         <v>0</v>
@@ -1437,30 +1437,30 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="n">
+      <c r="A44" s="1" t="n">
         <v>194943</v>
       </c>
       <c r="B44" t="n">
         <v>0</v>
       </c>
       <c r="C44" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E44" t="n">
         <v>0</v>
       </c>
       <c r="F44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G44" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="n">
+      <c r="A45" s="1" t="n">
         <v>195026</v>
       </c>
       <c r="B45" t="n">
@@ -1470,7 +1470,7 @@
         <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E45" t="n">
         <v>0</v>
@@ -1483,7 +1483,7 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="n">
+      <c r="A46" s="1" t="n">
         <v>216987</v>
       </c>
       <c r="B46" t="n">
@@ -1493,7 +1493,7 @@
         <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E46" t="n">
         <v>0</v>
@@ -1506,7 +1506,7 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="n">
+      <c r="A47" s="1" t="n">
         <v>191056</v>
       </c>
       <c r="B47" t="n">
@@ -1519,50 +1519,50 @@
         <v>0</v>
       </c>
       <c r="E47" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F47" t="n">
         <v>0</v>
       </c>
       <c r="G47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="n">
+      <c r="A48" s="1" t="n">
         <v>193406</v>
       </c>
       <c r="B48" t="n">
         <v>0</v>
       </c>
       <c r="C48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D48" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E48" t="n">
         <v>0</v>
       </c>
       <c r="F48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="n">
+      <c r="A49" s="1" t="n">
         <v>194028</v>
       </c>
       <c r="B49" t="n">
         <v>0</v>
       </c>
       <c r="C49" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E49" t="n">
         <v>0</v>
@@ -1571,41 +1571,41 @@
         <v>0</v>
       </c>
       <c r="G49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="n">
+      <c r="A50" s="1" t="n">
         <v>202255</v>
       </c>
       <c r="B50" t="n">
         <v>0</v>
       </c>
       <c r="C50" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E50" t="n">
         <v>0</v>
       </c>
       <c r="F50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G50" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="n">
+      <c r="A51" s="1" t="n">
         <v>39371</v>
       </c>
       <c r="B51" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D51" t="n">
         <v>0</v>
@@ -1621,7 +1621,7 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="n">
+      <c r="A52" s="1" t="n">
         <v>185410</v>
       </c>
       <c r="B52" t="n">
@@ -1634,17 +1634,17 @@
         <v>0</v>
       </c>
       <c r="E52" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F52" t="n">
         <v>0</v>
       </c>
       <c r="G52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="n">
+      <c r="A53" s="1" t="n">
         <v>214542</v>
       </c>
       <c r="B53" t="n">
@@ -1657,7 +1657,7 @@
         <v>0</v>
       </c>
       <c r="E53" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F53" t="n">
         <v>0</v>
@@ -1667,14 +1667,14 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="n">
+      <c r="A54" s="1" t="n">
         <v>183012</v>
       </c>
       <c r="B54" t="n">
         <v>0</v>
       </c>
       <c r="C54" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D54" t="n">
         <v>0</v>
@@ -1683,24 +1683,24 @@
         <v>0</v>
       </c>
       <c r="F54" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G54" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="n">
+      <c r="A55" s="1" t="n">
         <v>174454</v>
       </c>
       <c r="B55" t="n">
         <v>0</v>
       </c>
       <c r="C55" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E55" t="n">
         <v>0</v>
@@ -1709,34 +1709,34 @@
         <v>0</v>
       </c>
       <c r="G55" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="n">
+      <c r="A56" s="1" t="n">
         <v>185019</v>
       </c>
       <c r="B56" t="n">
         <v>0</v>
       </c>
       <c r="C56" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E56" t="n">
         <v>0</v>
       </c>
       <c r="F56" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="n">
+      <c r="A57" s="1" t="n">
         <v>173459</v>
       </c>
       <c r="B57" t="n">
@@ -1749,7 +1749,7 @@
         <v>0</v>
       </c>
       <c r="E57" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F57" t="n">
         <v>0</v>
@@ -1759,7 +1759,7 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="n">
+      <c r="A58" s="1" t="n">
         <v>16170</v>
       </c>
       <c r="B58" t="n">
@@ -1772,7 +1772,7 @@
         <v>0</v>
       </c>
       <c r="E58" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F58" t="n">
         <v>0</v>
@@ -1782,14 +1782,14 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="n">
+      <c r="A59" s="1" t="n">
         <v>200672</v>
       </c>
       <c r="B59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C59" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D59" t="n">
         <v>0</v>
@@ -1798,18 +1798,18 @@
         <v>0</v>
       </c>
       <c r="F59" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G59" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="n">
+      <c r="A60" s="1" t="n">
         <v>166772</v>
       </c>
       <c r="B60" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C60" t="n">
         <v>0</v>
@@ -1818,17 +1818,17 @@
         <v>0</v>
       </c>
       <c r="E60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F60" t="n">
         <v>0</v>
       </c>
       <c r="G60" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="n">
+      <c r="A61" s="1" t="n">
         <v>159438</v>
       </c>
       <c r="B61" t="n">
@@ -1838,10 +1838,10 @@
         <v>0</v>
       </c>
       <c r="D61" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F61" t="n">
         <v>0</v>
@@ -1851,14 +1851,14 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="n">
+      <c r="A62" s="1" t="n">
         <v>21935</v>
       </c>
       <c r="B62" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C62" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D62" t="n">
         <v>0</v>
@@ -1870,18 +1870,18 @@
         <v>0</v>
       </c>
       <c r="G62" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="n">
+      <c r="A63" s="1" t="n">
         <v>210751</v>
       </c>
       <c r="B63" t="n">
         <v>0</v>
       </c>
       <c r="C63" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D63" t="n">
         <v>0</v>
@@ -1890,14 +1890,14 @@
         <v>0</v>
       </c>
       <c r="F63" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G63" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="n">
+      <c r="A64" s="1" t="n">
         <v>163086</v>
       </c>
       <c r="B64" t="n">
@@ -1910,7 +1910,7 @@
         <v>0</v>
       </c>
       <c r="E64" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F64" t="n">
         <v>0</v>
@@ -1920,57 +1920,57 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="n">
+      <c r="A65" s="1" t="n">
         <v>217380</v>
       </c>
       <c r="B65" t="n">
         <v>0</v>
       </c>
       <c r="C65" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D65" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E65" t="n">
         <v>0</v>
       </c>
       <c r="F65" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G65" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="n">
+      <c r="A66" s="1" t="n">
         <v>210978</v>
       </c>
       <c r="B66" t="n">
         <v>0</v>
       </c>
       <c r="C66" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D66" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E66" t="n">
         <v>0</v>
       </c>
       <c r="F66" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G66" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="n">
+      <c r="A67" s="1" t="n">
         <v>170972</v>
       </c>
       <c r="B67" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C67" t="n">
         <v>0</v>
@@ -1979,17 +1979,17 @@
         <v>0</v>
       </c>
       <c r="E67" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F67" t="n">
         <v>0</v>
       </c>
       <c r="G67" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="n">
+      <c r="A68" s="1" t="n">
         <v>158658</v>
       </c>
       <c r="B68" t="n">
@@ -2002,7 +2002,7 @@
         <v>0</v>
       </c>
       <c r="E68" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F68" t="n">
         <v>0</v>
@@ -2012,11 +2012,11 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="n">
+      <c r="A69" s="1" t="n">
         <v>202892</v>
       </c>
       <c r="B69" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C69" t="n">
         <v>0</v>
@@ -2025,7 +2025,7 @@
         <v>0</v>
       </c>
       <c r="E69" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F69" t="n">
         <v>0</v>
@@ -2035,11 +2035,11 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="n">
+      <c r="A70" s="1" t="n">
         <v>99368</v>
       </c>
       <c r="B70" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C70" t="n">
         <v>0</v>
@@ -2054,21 +2054,21 @@
         <v>0</v>
       </c>
       <c r="G70" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="n">
+      <c r="A71" s="1" t="n">
         <v>218080</v>
       </c>
       <c r="B71" t="n">
         <v>0</v>
       </c>
       <c r="C71" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D71" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E71" t="n">
         <v>0</v>
@@ -2077,15 +2077,15 @@
         <v>0</v>
       </c>
       <c r="G71" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="n">
+      <c r="A72" s="1" t="n">
         <v>182686</v>
       </c>
       <c r="B72" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C72" t="n">
         <v>0</v>
@@ -2104,14 +2104,14 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="n">
+      <c r="A73" s="1" t="n">
         <v>82863</v>
       </c>
       <c r="B73" t="n">
         <v>0</v>
       </c>
       <c r="C73" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D73" t="n">
         <v>0</v>
@@ -2120,21 +2120,21 @@
         <v>0</v>
       </c>
       <c r="F73" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G73" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="n">
+      <c r="A74" s="1" t="n">
         <v>159710</v>
       </c>
       <c r="B74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C74" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D74" t="n">
         <v>0</v>
@@ -2143,14 +2143,14 @@
         <v>0</v>
       </c>
       <c r="F74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="n">
+      <c r="A75" s="1" t="n">
         <v>214075</v>
       </c>
       <c r="B75" t="n">
@@ -2163,67 +2163,67 @@
         <v>0</v>
       </c>
       <c r="E75" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F75" t="n">
         <v>0</v>
       </c>
       <c r="G75" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="n">
+      <c r="A76" s="1" t="n">
         <v>187340</v>
       </c>
       <c r="B76" t="n">
         <v>0</v>
       </c>
       <c r="C76" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D76" t="n">
         <v>0</v>
       </c>
       <c r="E76" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F76" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G76" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77" t="n">
+      <c r="A77" s="1" t="n">
         <v>166102</v>
       </c>
       <c r="B77" t="n">
         <v>0</v>
       </c>
       <c r="C77" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D77" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E77" t="n">
         <v>0</v>
       </c>
       <c r="F77" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G77" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78">
-      <c r="A78" t="n">
+      <c r="A78" s="1" t="n">
         <v>174818</v>
       </c>
       <c r="B78" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C78" t="n">
         <v>0</v>
@@ -2232,17 +2232,17 @@
         <v>0</v>
       </c>
       <c r="E78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F78" t="n">
         <v>0</v>
       </c>
       <c r="G78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79">
-      <c r="A79" t="n">
+      <c r="A79" s="1" t="n">
         <v>179465</v>
       </c>
       <c r="B79" t="n">
@@ -2255,17 +2255,17 @@
         <v>0</v>
       </c>
       <c r="E79" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F79" t="n">
         <v>0</v>
       </c>
       <c r="G79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80">
-      <c r="A80" t="n">
+      <c r="A80" s="1" t="n">
         <v>174451</v>
       </c>
       <c r="B80" t="n">
@@ -2278,17 +2278,17 @@
         <v>0</v>
       </c>
       <c r="E80" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F80" t="n">
         <v>0</v>
       </c>
       <c r="G80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81">
-      <c r="A81" t="n">
+      <c r="A81" s="1" t="n">
         <v>185290</v>
       </c>
       <c r="B81" t="n">
@@ -2301,7 +2301,7 @@
         <v>0</v>
       </c>
       <c r="E81" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F81" t="n">
         <v>0</v>
@@ -2311,14 +2311,14 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" t="n">
+      <c r="A82" s="1" t="n">
         <v>198316</v>
       </c>
       <c r="B82" t="n">
         <v>0</v>
       </c>
       <c r="C82" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D82" t="n">
         <v>0</v>
@@ -2327,14 +2327,14 @@
         <v>0</v>
       </c>
       <c r="F82" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G82" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="n">
+      <c r="A83" s="1" t="n">
         <v>158273</v>
       </c>
       <c r="B83" t="n">
@@ -2347,24 +2347,24 @@
         <v>0</v>
       </c>
       <c r="E83" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F83" t="n">
         <v>0</v>
       </c>
       <c r="G83" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="n">
+      <c r="A84" s="1" t="n">
         <v>150026</v>
       </c>
       <c r="B84" t="n">
         <v>0</v>
       </c>
       <c r="C84" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D84" t="n">
         <v>0</v>
@@ -2376,41 +2376,41 @@
         <v>0</v>
       </c>
       <c r="G84" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85">
-      <c r="A85" t="n">
+      <c r="A85" s="1" t="n">
         <v>216843</v>
       </c>
       <c r="B85" t="n">
         <v>0</v>
       </c>
       <c r="C85" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D85" t="n">
         <v>0</v>
       </c>
       <c r="E85" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F85" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G85" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86">
-      <c r="A86" t="n">
+      <c r="A86" s="1" t="n">
         <v>218470</v>
       </c>
       <c r="B86" t="n">
         <v>0</v>
       </c>
       <c r="C86" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D86" t="n">
         <v>0</v>
@@ -2419,14 +2419,14 @@
         <v>0</v>
       </c>
       <c r="F86" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G86" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87">
-      <c r="A87" t="n">
+      <c r="A87" s="1" t="n">
         <v>175482</v>
       </c>
       <c r="B87" t="n">
@@ -2436,7 +2436,7 @@
         <v>0</v>
       </c>
       <c r="D87" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E87" t="n">
         <v>0</v>
@@ -2449,7 +2449,7 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" t="n">
+      <c r="A88" s="1" t="n">
         <v>186893</v>
       </c>
       <c r="B88" t="n">
@@ -2459,7 +2459,7 @@
         <v>0</v>
       </c>
       <c r="D88" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E88" t="n">
         <v>0</v>
@@ -2472,11 +2472,11 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" t="n">
+      <c r="A89" s="1" t="n">
         <v>175281</v>
       </c>
       <c r="B89" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C89" t="n">
         <v>0</v>
@@ -2485,40 +2485,40 @@
         <v>0</v>
       </c>
       <c r="E89" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F89" t="n">
         <v>0</v>
       </c>
       <c r="G89" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="90">
-      <c r="A90" t="n">
+      <c r="A90" s="1" t="n">
         <v>161056</v>
       </c>
       <c r="B90" t="n">
         <v>0</v>
       </c>
       <c r="C90" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D90" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E90" t="n">
         <v>0</v>
       </c>
       <c r="F90" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G90" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="91">
-      <c r="A91" t="n">
+      <c r="A91" s="1" t="n">
         <v>186512</v>
       </c>
       <c r="B91" t="n">
@@ -2531,17 +2531,17 @@
         <v>0</v>
       </c>
       <c r="E91" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F91" t="n">
         <v>0</v>
       </c>
       <c r="G91" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92">
-      <c r="A92" t="n">
+      <c r="A92" s="1" t="n">
         <v>187956</v>
       </c>
       <c r="B92" t="n">
@@ -2554,7 +2554,7 @@
         <v>0</v>
       </c>
       <c r="E92" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F92" t="n">
         <v>0</v>
@@ -2564,14 +2564,14 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" t="n">
+      <c r="A93" s="1" t="n">
         <v>175485</v>
       </c>
       <c r="B93" t="n">
         <v>0</v>
       </c>
       <c r="C93" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D93" t="n">
         <v>0</v>
@@ -2580,14 +2580,14 @@
         <v>0</v>
       </c>
       <c r="F93" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G93" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94">
-      <c r="A94" t="n">
+      <c r="A94" s="1" t="n">
         <v>186275</v>
       </c>
       <c r="B94" t="n">
@@ -2600,7 +2600,7 @@
         <v>0</v>
       </c>
       <c r="E94" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F94" t="n">
         <v>0</v>
@@ -2610,11 +2610,11 @@
       </c>
     </row>
     <row r="95">
-      <c r="A95" t="n">
+      <c r="A95" s="1" t="n">
         <v>177410</v>
       </c>
       <c r="B95" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C95" t="n">
         <v>0</v>
@@ -2623,21 +2623,21 @@
         <v>0</v>
       </c>
       <c r="E95" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F95" t="n">
         <v>0</v>
       </c>
       <c r="G95" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96">
-      <c r="A96" t="n">
+      <c r="A96" s="1" t="n">
         <v>187563</v>
       </c>
       <c r="B96" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C96" t="n">
         <v>0</v>
@@ -2646,17 +2646,17 @@
         <v>0</v>
       </c>
       <c r="E96" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F96" t="n">
         <v>0</v>
       </c>
       <c r="G96" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97">
-      <c r="A97" t="n">
+      <c r="A97" s="1" t="n">
         <v>195041</v>
       </c>
       <c r="B97" t="n">
@@ -2666,7 +2666,7 @@
         <v>0</v>
       </c>
       <c r="D97" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E97" t="n">
         <v>0</v>
@@ -2679,7 +2679,7 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" t="n">
+      <c r="A98" s="1" t="n">
         <v>192115</v>
       </c>
       <c r="B98" t="n">
@@ -2689,7 +2689,7 @@
         <v>0</v>
       </c>
       <c r="D98" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E98" t="n">
         <v>0</v>
@@ -2702,7 +2702,7 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" t="n">
+      <c r="A99" s="1" t="n">
         <v>160011</v>
       </c>
       <c r="B99" t="n">
@@ -2715,7 +2715,7 @@
         <v>0</v>
       </c>
       <c r="E99" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F99" t="n">
         <v>0</v>
@@ -2725,30 +2725,30 @@
       </c>
     </row>
     <row r="100">
-      <c r="A100" t="n">
+      <c r="A100" s="1" t="n">
         <v>186532</v>
       </c>
       <c r="B100" t="n">
         <v>0</v>
       </c>
       <c r="C100" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D100" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E100" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F100" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G100" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="101">
-      <c r="A101" t="n">
+      <c r="A101" s="1" t="n">
         <v>166145</v>
       </c>
       <c r="B101" t="n">
@@ -2758,7 +2758,7 @@
         <v>0</v>
       </c>
       <c r="D101" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E101" t="n">
         <v>0</v>
@@ -2771,14 +2771,14 @@
       </c>
     </row>
     <row r="102">
-      <c r="A102" t="n">
+      <c r="A102" s="1" t="n">
         <v>213869</v>
       </c>
       <c r="B102" t="n">
         <v>0</v>
       </c>
       <c r="C102" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D102" t="n">
         <v>0</v>
@@ -2787,37 +2787,37 @@
         <v>0</v>
       </c>
       <c r="F102" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G102" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103">
-      <c r="A103" t="n">
+      <c r="A103" s="1" t="n">
         <v>175394</v>
       </c>
       <c r="B103" t="n">
         <v>0</v>
       </c>
       <c r="C103" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D103" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E103" t="n">
         <v>0</v>
       </c>
       <c r="F103" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G103" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="104">
-      <c r="A104" t="n">
+      <c r="A104" s="1" t="n">
         <v>173122</v>
       </c>
       <c r="B104" t="n">
@@ -2827,7 +2827,7 @@
         <v>0</v>
       </c>
       <c r="D104" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E104" t="n">
         <v>0</v>
@@ -2840,14 +2840,14 @@
       </c>
     </row>
     <row r="105">
-      <c r="A105" t="n">
+      <c r="A105" s="1" t="n">
         <v>162625</v>
       </c>
       <c r="B105" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C105" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D105" t="n">
         <v>0</v>
@@ -2859,34 +2859,34 @@
         <v>0</v>
       </c>
       <c r="G105" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="106">
-      <c r="A106" t="n">
+      <c r="A106" s="1" t="n">
         <v>212627</v>
       </c>
       <c r="B106" t="n">
         <v>0</v>
       </c>
       <c r="C106" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D106" t="n">
         <v>0</v>
       </c>
       <c r="E106" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F106" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G106" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107">
-      <c r="A107" t="n">
+      <c r="A107" s="1" t="n">
         <v>297473</v>
       </c>
       <c r="B107" t="n">
@@ -2899,7 +2899,7 @@
         <v>0</v>
       </c>
       <c r="E107" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F107" t="n">
         <v>0</v>
@@ -2909,7 +2909,7 @@
       </c>
     </row>
     <row r="108">
-      <c r="A108" t="n">
+      <c r="A108" s="1" t="n">
         <v>184693</v>
       </c>
       <c r="B108" t="n">
@@ -2922,7 +2922,7 @@
         <v>0</v>
       </c>
       <c r="E108" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F108" t="n">
         <v>0</v>
@@ -2932,11 +2932,11 @@
       </c>
     </row>
     <row r="109">
-      <c r="A109" t="n">
+      <c r="A109" s="1" t="n">
         <v>42276</v>
       </c>
       <c r="B109" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C109" t="n">
         <v>0</v>
@@ -2951,15 +2951,15 @@
         <v>0</v>
       </c>
       <c r="G109" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="110">
-      <c r="A110" t="n">
+      <c r="A110" s="1" t="n">
         <v>112989</v>
       </c>
       <c r="B110" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C110" t="n">
         <v>0</v>
@@ -2978,7 +2978,7 @@
       </c>
     </row>
     <row r="111">
-      <c r="A111" t="n">
+      <c r="A111" s="1" t="n">
         <v>6124</v>
       </c>
       <c r="B111" t="n">
@@ -2991,7 +2991,7 @@
         <v>0</v>
       </c>
       <c r="E111" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F111" t="n">
         <v>0</v>

</xml_diff>